<commit_message>
Test report and bug report added
</commit_message>
<xml_diff>
--- a/Docs/LFR-Form-TestCases.xlsx
+++ b/Docs/LFR-Form-TestCases.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasblooo\Desktop\Entrevista Liferay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasblooo\Desktop\EntrevistaLiferay\interview-liferay-form\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFA5D9D-4679-4109-A4C4-D8D058D4EA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABA43BD-BE3C-416E-B68E-367E537011E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35475" yWindow="30" windowWidth="31065" windowHeight="20205" xr2:uid="{54F0BD1D-40C6-499E-96D8-45F272A59A74}"/>
+    <workbookView xWindow="1125" yWindow="210" windowWidth="20835" windowHeight="20205" xr2:uid="{54F0BD1D-40C6-499E-96D8-45F272A59A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$M$36</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="148">
   <si>
     <t>Change region</t>
   </si>
@@ -81,9 +84,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Issue Type</t>
   </si>
   <si>
     <t>Severity</t>
@@ -393,13 +393,127 @@
   </si>
   <si>
     <t>https://forms.liferay.com/web/forms/shared/-/form/122548?p_p_state=pop_up&amp;p_p_auth=bsdX7ixp&amp;_com_liferay_dynamic_data_mapping_form_web_portlet_DDMFormPortlet_languageId=pt_BR</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Inform the user that there are characters not allowed in the Name field</t>
+  </si>
+  <si>
+    <t>Inform the user that the birth date cannot be in the future</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0001</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0002</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0003</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0004</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0005</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0006</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0007</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0008</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0009</t>
+  </si>
+  <si>
+    <t>LFR-FORM-BUG-0010</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Following the warning text is a numeric identifier that it should not. It could confuse the user. Observe the screenshot </t>
+  </si>
+  <si>
+    <t>Some texts appear in a language other than that of the region. Observe the screenshot</t>
+  </si>
+  <si>
+    <t>When the date of birth field is left unfilled, it does not warn the user until the submit button has been pressed. Look at the screenshot</t>
+  </si>
+  <si>
+    <t>Special characters should not be allowed on forms, in the absence of security tests, unless strictly necessary.</t>
+  </si>
+  <si>
+    <t>Being a date of birth, the form should validate that at least it is not a date in the future.</t>
+  </si>
+  <si>
+    <t>REGION-01</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0001</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0003</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0004</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0005</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0006</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0007</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0008</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0009</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0010</t>
+  </si>
+  <si>
+    <t>EVIDENCE-BUG-0002</t>
+  </si>
+  <si>
+    <t>The form for the Portuguese region does not allow the sending of the data unless in any case since an error is detected in the field of the date of birth.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +543,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +581,22 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,11 +769,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -637,9 +796,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -651,9 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -665,24 +818,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -693,8 +834,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1010,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142A1A7B-FA94-4D81-8C94-11EA3EDFF5B5}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,22 +1206,22 @@
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.28515625" customWidth="1"/>
     <col min="8" max="8" width="63.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.42578125" style="31" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>8</v>
@@ -1048,15 +1230,15 @@
         <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="30" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -1066,994 +1248,1252 @@
         <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="15"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="I3" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="23"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38"/>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="I4" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="23"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="M4" s="20"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38"/>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="I5" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="23"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38"/>
       <c r="B6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="I6" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38"/>
       <c r="B7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="I7" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="23"/>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="I8" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="23"/>
-    </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38"/>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="I9" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38"/>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="I10" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38"/>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="I11" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="23"/>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38"/>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="I12" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="23"/>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="M12" s="20"/>
+    </row>
+    <row r="13" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39"/>
+      <c r="B14" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="23"/>
-    </row>
-    <row r="14" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17" t="s">
+      <c r="I14" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="D15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="F15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39"/>
+      <c r="B16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E16" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F16" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="G16" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="I16" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="L16" s="18"/>
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F17" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="I17" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K17" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="21"/>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="25" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="I18" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
       <c r="B19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41"/>
       <c r="B20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="23"/>
-    </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="I20" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
       <c r="B21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="23"/>
-    </row>
-    <row r="22" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="41"/>
       <c r="B22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="23"/>
-    </row>
-    <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="41"/>
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="23"/>
-    </row>
-    <row r="24" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
       <c r="B24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J24" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="23"/>
-    </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
       <c r="B25" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="23"/>
-    </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+        <v>75</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
       <c r="B26" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="23"/>
-    </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+        <v>81</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
       <c r="B27" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="23"/>
-    </row>
-    <row r="28" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="I27" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
       <c r="B28" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="23"/>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="I28" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="J28" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
       <c r="B29" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J29" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="23"/>
-    </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="M29" s="20"/>
+    </row>
+    <row r="30" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
       <c r="B30" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="23"/>
-    </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L31" s="1"/>
-      <c r="M31" s="23"/>
-    </row>
-    <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="M31" s="20"/>
+    </row>
+    <row r="32" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="41"/>
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J32" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L32" s="1"/>
-      <c r="M32" s="23"/>
-    </row>
-    <row r="33" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="M32" s="20"/>
+    </row>
+    <row r="33" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="41"/>
       <c r="B33" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="I33" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J33" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="23"/>
-    </row>
-    <row r="34" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="M33" s="20"/>
+    </row>
+    <row r="34" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="41"/>
       <c r="B34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="I34" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="23"/>
-    </row>
-    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="41"/>
       <c r="B35" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="23"/>
+        <v>75</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J35" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="29" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="29"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="21"/>
+      <c r="H36" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I36" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="J36" s="26">
+        <v>44515</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M36" xr:uid="{142A1A7B-FA94-4D81-8C94-11EA3EDFF5B5}"/>
   <mergeCells count="3">
     <mergeCell ref="A2:A14"/>
     <mergeCell ref="A15:A16"/>
@@ -2063,9 +2503,10 @@
   <hyperlinks>
     <hyperlink ref="G15" r:id="rId1" xr:uid="{FC842FFF-5127-4D72-8B0A-39A043E0810D}"/>
     <hyperlink ref="G16" r:id="rId2" xr:uid="{681C6BAF-94E9-4CB5-B790-1A13959C3427}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{175CAB17-6722-4FA9-B20B-79183C23EAC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2073,14 +2514,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0147616-9BD4-41DE-BA33-A4907EBC7FB4}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -2089,7 +2532,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -2098,118 +2541,238 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+    <row r="3" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
@@ -2444,6 +3007,7 @@
       <c r="H34" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>